<commit_message>
Analisis de Datos, sigmas, nulos, etc.
</commit_message>
<xml_diff>
--- a/sensores_airenuevoleon.xlsx
+++ b/sensores_airenuevoleon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\SN3PEPF00017B75\EXCELCNV\f3042668-9cb4-488c-b34b-d1c36e35ce3b\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chavez/Desktop/daacc_preficient/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7338F104-C4DE-4C17-BA9A-DB123381A095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D4D03C-FE4E-1046-B0F4-2D663414445C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{97D38D6E-BA2E-4798-B6FA-CB53A456057F}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{97D38D6E-BA2E-4798-B6FA-CB53A456057F}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>Sensor_id</t>
   </si>
@@ -113,9 +113,6 @@
     <t>ANL13</t>
   </si>
   <si>
-    <t>JuÃ¡rez</t>
-  </si>
-  <si>
     <t>LAZARO GARZA AYALA ESQ. CON GRAL. SANTIAGO TAPIA</t>
   </si>
   <si>
@@ -125,36 +122,18 @@
     <t>Pesqueria</t>
   </si>
   <si>
-    <t>Boulevard Rogelio A. PÃ©rez Arrambide</t>
-  </si>
-  <si>
-    <t>PesquerÃ­a</t>
-  </si>
-  <si>
     <t>ANL16</t>
   </si>
   <si>
     <t>San Juan</t>
   </si>
   <si>
-    <t>Av. MisÃ³n Arcos 69, MisiÃ³n San Juan</t>
-  </si>
-  <si>
-    <t>GarcÃ­a</t>
-  </si>
-  <si>
     <t>ANL2</t>
   </si>
   <si>
-    <t>San NicolÃ¡s</t>
-  </si>
-  <si>
     <t>ANTONIO SOTO Y GAMMA ESQ. CON ALAMO</t>
   </si>
   <si>
-    <t>San NicolÃ¡s de los Garza</t>
-  </si>
-  <si>
     <t>ANL3</t>
   </si>
   <si>
@@ -170,15 +149,9 @@
     <t>San Pedro</t>
   </si>
   <si>
-    <t>GRAL. GARZA AYALA ESQUINA CON DIEGO SALDÃVAR</t>
-  </si>
-  <si>
     <t>ANL5</t>
   </si>
   <si>
-    <t>San NicolÃ¡s (UANL)</t>
-  </si>
-  <si>
     <t>CIUDAD UNIVERSITARIA, FAC CONTADURIA</t>
   </si>
   <si>
@@ -191,9 +164,6 @@
     <t>ANL7</t>
   </si>
   <si>
-    <t>San BernabÃ©</t>
-  </si>
-  <si>
     <t>PROL AZTLAN 9610, SAN BERNABE VIII SECTOR</t>
   </si>
   <si>
@@ -206,9 +176,6 @@
     <t>CAMPESINA CRUZ CON VICENTE GUERRERO</t>
   </si>
   <si>
-    <t>Cadereyta JimÃ©nez</t>
-  </si>
-  <si>
     <t>ANL9</t>
   </si>
   <si>
@@ -219,13 +186,49 @@
   </si>
   <si>
     <t>General Escobedo</t>
+  </si>
+  <si>
+    <t>Juarez</t>
+  </si>
+  <si>
+    <t>San Bernabé</t>
+  </si>
+  <si>
+    <t>García</t>
+  </si>
+  <si>
+    <t>San Nicolás</t>
+  </si>
+  <si>
+    <t>San Nicolás (UANL)</t>
+  </si>
+  <si>
+    <t>GRAL. GARZA AYALA ESQUINA CON DIEGO SALDÍVAR</t>
+  </si>
+  <si>
+    <t>Juárez</t>
+  </si>
+  <si>
+    <t>San Nicolás de los Garza</t>
+  </si>
+  <si>
+    <t>Cadereyta Jiménez</t>
+  </si>
+  <si>
+    <t>Pesquería</t>
+  </si>
+  <si>
+    <t>Boulevard Rogelio A. Pérez Arrambide</t>
+  </si>
+  <si>
+    <t>Av. Misión Arcos 69, Misión San Juan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -763,9 +766,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -803,7 +806,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -909,7 +912,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1051,7 +1054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1061,11 +1064,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CFFA9D2-8428-4685-8735-399150EC3D6A}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="48.33203125" customWidth="1"/>
+    <col min="4" max="4" width="29" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1135,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1170,7 +1180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1205,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1240,18 +1250,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="E6">
         <v>67250</v>
@@ -1275,18 +1285,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E7">
         <v>66650</v>
@@ -1310,18 +1320,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E8">
         <v>66023</v>
@@ -1345,18 +1355,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E9">
         <v>66440</v>
@@ -1380,18 +1390,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E10">
         <v>66350</v>
@@ -1415,18 +1425,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E11">
         <v>66280</v>
@@ -1450,18 +1460,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="E12">
         <v>66451</v>
@@ -1485,18 +1495,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E13">
         <v>66004</v>
@@ -1520,15 +1530,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -1555,18 +1565,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E15">
         <v>67483</v>
@@ -1590,18 +1600,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E16">
         <v>66070</v>

</xml_diff>